<commit_message>
added the eeprom.h file in project, updated the singl sample_app xls file.
</commit_message>
<xml_diff>
--- a/etherCAT_Apps/EVB_LAN9255_SIP_E53/EVB_LAN9255_SIP_E53/sample_app.xlsx
+++ b/etherCAT_Apps/EVB_LAN9255_SIP_E53/EVB_LAN9255_SIP_E53/sample_app.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\J2_SIP\same53_ssc\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3633E6D4-7A67-4BD9-A084-C56144E5392E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7637E7B1-3A28-46AF-B02F-38F1B4B79F43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -17,8 +17,8 @@
     <sheet name="Profile" sheetId="11" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Profile!$B$10:$P$68</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Profile!$B$1:$P$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Profile!$B$10:$P$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Profile!$B$1:$P$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
   <si>
     <t>Index</t>
   </si>
@@ -406,12 +406,6 @@
   </si>
   <si>
     <t>rx_ready</t>
-  </si>
-  <si>
-    <t>pad_7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                    </t>
   </si>
 </sst>
 </file>
@@ -895,11 +889,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T921"/>
+  <dimension ref="A1:T920"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
+      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -1727,8 +1721,8 @@
       <c r="D38" s="16">
         <v>2</v>
       </c>
-      <c r="E38" s="16" t="s">
-        <v>63</v>
+      <c r="E38" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>79</v>
@@ -1739,8 +1733,8 @@
       <c r="H38" s="16">
         <v>0</v>
       </c>
-      <c r="I38" s="16" t="s">
-        <v>77</v>
+      <c r="I38" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="L38" s="16" t="s">
         <v>48</v>
@@ -1753,12 +1747,8 @@
       <c r="A39" s="13"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
-      <c r="D39" s="16">
-        <v>3</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>78</v>
-      </c>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
@@ -1766,9 +1756,7 @@
       <c r="J39" s="16"/>
       <c r="K39" s="16"/>
       <c r="L39" s="16"/>
-      <c r="M39" s="16" t="s">
-        <v>50</v>
-      </c>
+      <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
       <c r="P39" s="16"/>
@@ -1777,12 +1765,8 @@
       <c r="A40" s="13"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
-      <c r="D40" s="16">
-        <v>4</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>75</v>
-      </c>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
@@ -1790,9 +1774,7 @@
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
       <c r="L40" s="16"/>
-      <c r="M40" s="16" t="s">
-        <v>50</v>
-      </c>
+      <c r="M40" s="16"/>
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
       <c r="P40" s="16"/>
@@ -1832,8 +1814,8 @@
       <c r="D43" s="22">
         <v>1</v>
       </c>
-      <c r="E43" s="18" t="s">
-        <v>64</v>
+      <c r="E43" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>82</v>
@@ -1855,194 +1837,185 @@
       </c>
       <c r="P43" s="18"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A44" s="4"/>
-      <c r="D44" s="16">
-        <v>2</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="M44" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="P44" s="18"/>
+    <row r="44" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="13"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
-      <c r="D45" s="16">
-        <v>3</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>84</v>
-      </c>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
       <c r="G45" s="16"/>
       <c r="H45" s="16"/>
       <c r="I45" s="16"/>
       <c r="J45" s="16"/>
       <c r="K45" s="16"/>
       <c r="L45" s="16"/>
-      <c r="M45" s="16" t="s">
-        <v>50</v>
-      </c>
+      <c r="M45" s="16"/>
       <c r="N45" s="16"/>
       <c r="O45" s="16"/>
     </row>
-    <row r="46" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="13"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16">
-        <v>4</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="16"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="16"/>
-      <c r="M46" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="N46" s="16"/>
-      <c r="O46" s="16"/>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="13"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="13"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A48" s="4"/>
-      <c r="B48" s="14" t="s">
+      <c r="B47" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C47" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-    </row>
-    <row r="49" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="13"/>
-      <c r="B49" s="4" t="s">
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+    </row>
+    <row r="48" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="13"/>
+      <c r="B48" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="13"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="11">
+        <v>1</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="F49" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
+        <v>62</v>
+      </c>
+      <c r="G49" s="21">
+        <v>0</v>
+      </c>
+      <c r="H49" s="21">
+        <v>0</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>58</v>
+      </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="M49" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
       <c r="P49" s="13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="11">
-        <v>1</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F50" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G50" s="21">
+      <c r="D50" s="22">
+        <v>2</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G50" s="16">
         <v>0</v>
       </c>
-      <c r="H50" s="21">
+      <c r="H50" s="16">
         <v>0</v>
       </c>
-      <c r="I50" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="20" t="s">
+      <c r="I50" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="L50" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="M50" s="4" t="s">
+      <c r="M50" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-      <c r="P50" s="13" t="s">
-        <v>60</v>
-      </c>
+      <c r="P50" s="13"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
       <c r="D51" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="F51" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="G51" s="16">
-        <v>0</v>
-      </c>
-      <c r="H51" s="16">
-        <v>0</v>
-      </c>
-      <c r="I51" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="L51" s="24" t="s">
-        <v>49</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="L51" s="24"/>
       <c r="M51" s="16" t="s">
         <v>47</v>
       </c>
@@ -2051,10 +2024,10 @@
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="4"/>
       <c r="D52" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F52" s="18"/>
       <c r="G52" s="18"/>
@@ -2068,102 +2041,112 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" s="4"/>
-      <c r="D53" s="22">
-        <v>4</v>
-      </c>
-      <c r="E53" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="L53" s="24"/>
-      <c r="M53" s="16" t="s">
-        <v>47</v>
-      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
       <c r="P53" s="13"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="13"/>
-    </row>
-    <row r="55" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="13"/>
-      <c r="B55" s="14" t="s">
+    <row r="54" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="13"/>
+      <c r="B54" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C54" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
-      <c r="P55" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A55" s="4"/>
+      <c r="B55" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="22"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="L55" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="P55" s="18"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" s="4"/>
-      <c r="B56" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D56" s="22"/>
-      <c r="E56" s="18"/>
+      <c r="D56" s="22">
+        <v>1</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>51</v>
+      </c>
       <c r="F56" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="L56" s="24" t="s">
-        <v>48</v>
+        <v>67</v>
+      </c>
+      <c r="G56" s="23">
+        <v>9600</v>
+      </c>
+      <c r="H56" s="23">
+        <v>0</v>
+      </c>
+      <c r="I56" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="L56" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="M56" s="16" t="s">
+        <v>47</v>
       </c>
       <c r="P56" s="18"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A57" s="4"/>
       <c r="D57" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F57" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G57" s="23">
-        <v>9600</v>
+        <v>0</v>
       </c>
       <c r="H57" s="23">
         <v>0</v>
       </c>
-      <c r="I57" s="18" t="s">
-        <v>53</v>
+      <c r="I57" s="23">
+        <v>3</v>
       </c>
       <c r="L57" s="16" t="s">
         <v>49</v>
@@ -2171,27 +2154,29 @@
       <c r="M57" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="P57" s="18"/>
-    </row>
-    <row r="58" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="P57" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" s="4"/>
       <c r="D58" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G58" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" s="23">
         <v>0</v>
       </c>
       <c r="I58" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L58" s="16" t="s">
         <v>49</v>
@@ -2199,23 +2184,21 @@
       <c r="M58" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="P58" s="25" t="s">
-        <v>69</v>
-      </c>
+      <c r="P58" s="18"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="4"/>
       <c r="D59" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E59" s="18" t="s">
         <v>64</v>
       </c>
       <c r="F59" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G59" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59" s="23">
         <v>0</v>
@@ -2231,16 +2214,16 @@
       </c>
       <c r="P59" s="18"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="4"/>
       <c r="D60" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E60" s="18" t="s">
         <v>64</v>
       </c>
       <c r="F60" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G60" s="23">
         <v>0</v>
@@ -2257,65 +2240,57 @@
       <c r="M60" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="P60" s="18"/>
-    </row>
-    <row r="61" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="P60" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" s="4"/>
       <c r="D61" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F61" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G61" s="23">
-        <v>0</v>
-      </c>
-      <c r="H61" s="23">
-        <v>0</v>
-      </c>
-      <c r="I61" s="23">
-        <v>1</v>
-      </c>
-      <c r="L61" s="16" t="s">
-        <v>49</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
       <c r="M61" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="P61" s="25" t="s">
-        <v>73</v>
-      </c>
+      <c r="P61" s="18"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="4"/>
-      <c r="D62" s="22">
-        <v>6</v>
-      </c>
-      <c r="E62" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="11">
+        <v>7</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
       <c r="M62" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="P62" s="18"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="13"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
-      <c r="D63" s="11">
-        <v>7</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>75</v>
-      </c>
+      <c r="D63" s="11"/>
+      <c r="E63" s="13"/>
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
       <c r="H63" s="13"/>
@@ -2323,52 +2298,50 @@
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="16" t="s">
-        <v>47</v>
-      </c>
+      <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
       <c r="P63" s="13"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
-      <c r="P64" s="13"/>
+      <c r="B64" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="14"/>
+      <c r="P64" s="14"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="4"/>
-      <c r="B65" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
-      <c r="O65" s="14"/>
-      <c r="P65" s="14"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4"/>
+      <c r="P65" s="13"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="4"/>
@@ -2389,43 +2362,42 @@
       <c r="P66" s="13"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-      <c r="P67" s="13"/>
+      <c r="B67" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="14"/>
+      <c r="N67" s="14"/>
+      <c r="O67" s="14"/>
+      <c r="P67" s="14"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B68" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C68" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-      <c r="K68" s="14"/>
-      <c r="L68" s="14"/>
-      <c r="M68" s="14"/>
-      <c r="N68" s="14"/>
-      <c r="O68" s="14"/>
-      <c r="P68" s="14"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="13"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B69" s="4"/>
@@ -2447,19 +2419,19 @@
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
       <c r="N70" s="4"/>
       <c r="O70" s="4"/>
-      <c r="P70" s="13"/>
+      <c r="P70" s="4"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B71" s="4"/>
@@ -2631,66 +2603,52 @@
       <c r="O80" s="4"/>
       <c r="P80" s="4"/>
     </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B81" s="4"/>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="4"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
-      <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
-    </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C82" s="4"/>
     </row>
-    <row r="83" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C84" s="4"/>
     </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C85" s="4"/>
     </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C86" s="4"/>
     </row>
-    <row r="87" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C87" s="4"/>
     </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C88" s="4"/>
     </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C89" s="4"/>
     </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C91" s="4"/>
     </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C96" s="4"/>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.35">
@@ -5165,31 +5123,28 @@
     <row r="920" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C920" s="4"/>
     </row>
-    <row r="921" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C921" s="4"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatRows="0" insertRows="0" insertHyperlinks="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="B10:P68" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B10:P67" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="F1:P6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C82:C921" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C81:C920" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"VARIABLE,ARRAY,RECORD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M12:O13 M15:O16 M18:O19 M21:O22 M27:O28 M30:O31 M33:O34 M56:O64 M66:O67 M69:O70 M24:O25 M36:O37 M47:O47 M49:O54 N43:O46" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M12:O13 M15:O16 M18:O19 M21:O22 M27:O28 M30:O31 M33:O34 M55:O63 M65:O66 M68:O69 M24:O25 M36:O37 M46:O46 M48:O53 N43:O45" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"rx,tx"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Object Code value" error="The Object code value shall be:_x000a_VARIABLE_x000a_RECORD_x000a_ARRAY" sqref="C12:C13 C15:C16 C18:C19 C21:C22 C27:C28 C30:C31 C33:C34 C66:C67 C69:C81 C24:C25 C36:C41 C49:C54 C56:C64 C43:C47" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Object Code value" error="The Object code value shall be:_x000a_VARIABLE_x000a_RECORD_x000a_ARRAY" sqref="C12:C13 C15:C16 C18:C19 C21:C22 C27:C28 C30:C31 C33:C34 C65:C66 C68:C80 C24:C25 C36:C41 C48:C53 C55:C63 C43:C46" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"VARIABLE,ARRAY,RECORD"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="C11 C14 C17 C20 C23 C26 C29 C32 C68 C48 C65 C35 C55" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Category" error="The value for the entry category shall be _x000a_M : (mandatory)_x000a_O : (optional) _x000a_C : (conditional)" sqref="J12:J13 J15:J16 J18:J19 J21:J22 J27:J28 J30:J31 J33:J34 J66:J67 J69:J81 J24:J25 J36:J37 J47 J49:J54 J56:J64 J43" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="C11 C14 C17 C20 C23 C26 C29 C32 C67 C47 C64 C35 C54" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Category" error="The value for the entry category shall be _x000a_M : (mandatory)_x000a_O : (optional) _x000a_C : (conditional)" sqref="J12:J13 J15:J16 J18:J19 J21:J22 J27:J28 J30:J31 J33:J34 J65:J66 J68:J80 J24:J25 J36:J37 J46 J48:J53 J55:J63 J43" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"M,O,C"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Backup/Setting Flag" error="The entry flag shall be_x000a_B : (Backup)_x000a_S : (Setting)" sqref="K12:K13 K15:K16 K18:K19 K21:K22 K27:K28 K30:K31 K33:K34 K66:K67 K69:K81 K24:K25 K36:K37 K47 K49:K54 K56:K64 K43" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Backup/Setting Flag" error="The entry flag shall be_x000a_B : (Backup)_x000a_S : (Setting)" sqref="K12:K13 K15:K16 K18:K19 K21:K22 K27:K28 K30:K31 K33:K34 K65:K66 K68:K80 K24:K25 K36:K37 K46 K48:K53 K55:K63 K43" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"B,S"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>